<commit_message>
Meer experimenteerwerk met parallelStream.forEach
*parallelStream.forEach() in f_addDefaultEnergyAssets ongedaan gemaakt; geeft onvoorspelbaar gedrag en is niet sneller (op mijn laptop iig)
*parallellisatie in hoofd tijdstap-event alleen op de populatie gridConnections (for now...) Dat is verreweg de zwaarste stap.
*Parameter toegevoegd p_paralellize waarmee parallelisatie aan en uit gezet kan worden, toegevoegd aan cloud-model inputs
*Parameter p_importLocalJsonConfigs toegevoegd aan cloud-model inputs, zodat die in de cloud altijd op False geforceerd kan worden (tenzij je dat niet wil natuurlijk)
*Python class Experiment uitgebreid met parallelize parameter
</commit_message>
<xml_diff>
--- a/Base/APIOutputRunData_1000_gridConnections.xlsx
+++ b/Base/APIOutputRunData_1000_gridConnections.xlsx
@@ -526,77 +526,77 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>8761</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>8760.0</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>13.806</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>5739</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>968</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
           <t>0</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>8760.0</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>0.439</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>0.007</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>5726</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>968</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>586.595</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>48258.307</t>
         </is>
       </c>
     </row>

</xml_diff>